<commit_message>
out of limit flags added
</commit_message>
<xml_diff>
--- a/КУМП.xlsx
+++ b/КУМП.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>0x1</t>
   </si>
@@ -73,13 +73,54 @@
   </si>
   <si>
     <t xml:space="preserve">CRCE (CRC Error) . CRCE = 1 если расчётная контрольная сумма для температуры или влажности не соответствует принятой по интерфейсу i2c. В этом случае в регистрах "Давление" и "Влажность" остаются предыдущие значения с верной CRC.  Флаг снимается после получения корректной контрольной суммы вместе с новыми значениями температуры и влажности. </t>
+  </si>
+  <si>
+    <t>HOL (Humidity out of limits) - превышение допустимых пределов измерений Влажности.  HOL = 1, если полученное значение влажности не входит в допустимый диапазон измерений (0-100%).</t>
+  </si>
+  <si>
+    <t>POL (Pressure out of limits) - превышение допустимых пределов измерений давления.  POL = 1, если полученное значение давления не входит в допустимый диапазон измерений (20.26 кПА - 405.2 кПА).</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>TOL</t>
+  </si>
+  <si>
+    <t>HOL</t>
+  </si>
+  <si>
+    <r>
+      <t>TOL (Temperature out of limits) - превышение допустимых пределов измерений Температуры. TOL = 1, если полученное значение температуры не входит в допустимый диапазон измерений (-40</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>°с</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - 125°с).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +145,13 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -578,7 +626,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -621,25 +669,67 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -666,72 +756,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1033,10 +1082,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R45"/>
+  <dimension ref="A2:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,69 +1097,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="29"/>
-      <c r="O13" s="29"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="30"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="44"/>
     </row>
     <row r="14" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="19"/>
-      <c r="B14" s="25" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="27"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="41"/>
       <c r="P14" s="1">
         <v>0</v>
       </c>
@@ -1320,151 +1369,163 @@
     </row>
     <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="31">
         <v>15</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D30" s="31">
         <v>14</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="31">
         <v>13</v>
       </c>
-      <c r="F30" s="20">
+      <c r="F30" s="31">
         <v>12</v>
       </c>
-      <c r="G30" s="20">
+      <c r="G30" s="31">
         <v>11</v>
       </c>
-      <c r="H30" s="20">
+      <c r="H30" s="31">
         <v>10</v>
       </c>
-      <c r="I30" s="20">
+      <c r="I30" s="31">
         <v>9</v>
       </c>
-      <c r="J30" s="20">
+      <c r="J30" s="31">
         <v>8</v>
       </c>
-      <c r="K30" s="20">
+      <c r="K30" s="31">
         <v>7</v>
       </c>
-      <c r="L30" s="20">
+      <c r="L30" s="31">
         <v>6</v>
       </c>
-      <c r="M30" s="20">
+      <c r="M30" s="31">
         <v>5</v>
       </c>
-      <c r="N30" s="20">
+      <c r="N30" s="31">
         <v>4</v>
       </c>
-      <c r="O30" s="20">
+      <c r="O30" s="31">
         <v>3</v>
       </c>
-      <c r="P30" s="20">
+      <c r="P30" s="31">
         <v>2</v>
       </c>
-      <c r="Q30" s="20">
+      <c r="Q30" s="31">
         <v>1</v>
       </c>
-      <c r="R30" s="34">
+      <c r="R30" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="32"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="21"/>
-      <c r="N31" s="21"/>
-      <c r="O31" s="21"/>
-      <c r="P31" s="21"/>
-      <c r="Q31" s="21"/>
-      <c r="R31" s="35"/>
+      <c r="A31" s="45"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="27"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="33"/>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="22"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="22"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="22"/>
-      <c r="P32" s="22"/>
-      <c r="Q32" s="22"/>
-      <c r="R32" s="36"/>
+      <c r="A32" s="46"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="34"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34"/>
+      <c r="N32" s="34"/>
+      <c r="O32" s="34"/>
+      <c r="P32" s="34"/>
+      <c r="Q32" s="34"/>
+      <c r="R32" s="28"/>
     </row>
     <row r="33" spans="1:18" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="51" t="s">
+      <c r="C33" s="18"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="N33" s="50" t="s">
+        <v>22</v>
+      </c>
+      <c r="O33" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="P33" s="50" t="s">
         <v>17</v>
       </c>
       <c r="Q33" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="R33" s="17" t="s">
+      <c r="R33" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="40"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="47"/>
-      <c r="D34" s="48"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
-      <c r="I34" s="48"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="48"/>
-      <c r="L34" s="48"/>
-      <c r="M34" s="48"/>
-      <c r="N34" s="48"/>
-      <c r="O34" s="48"/>
-      <c r="P34" s="52">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="16">
+      <c r="A34" s="30"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="25">
+        <v>0</v>
+      </c>
+      <c r="N34" s="51">
+        <v>0</v>
+      </c>
+      <c r="O34" s="51">
+        <v>0</v>
+      </c>
+      <c r="P34" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="17">
         <v>1</v>
       </c>
       <c r="R34" s="13">
@@ -1508,22 +1569,22 @@
       <c r="L35" s="11">
         <v>0</v>
       </c>
-      <c r="M35" s="11">
-        <v>0</v>
-      </c>
-      <c r="N35" s="11">
-        <v>0</v>
-      </c>
-      <c r="O35" s="11">
-        <v>0</v>
-      </c>
-      <c r="P35" s="49">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="49">
-        <v>0</v>
-      </c>
-      <c r="R35" s="50">
+      <c r="M35" s="22">
+        <v>0</v>
+      </c>
+      <c r="N35" s="22">
+        <v>0</v>
+      </c>
+      <c r="O35" s="22">
+        <v>0</v>
+      </c>
+      <c r="P35" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="22">
+        <v>0</v>
+      </c>
+      <c r="R35" s="23">
         <v>0</v>
       </c>
     </row>
@@ -1661,86 +1722,242 @@
     </row>
     <row r="40" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:18" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="42" t="s">
+      <c r="A41" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="43"/>
-      <c r="C41" s="43"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="43"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="43"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="43"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="43"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="43"/>
-      <c r="N41" s="43"/>
-      <c r="O41" s="43"/>
-      <c r="P41" s="43"/>
-      <c r="Q41" s="43"/>
-      <c r="R41" s="44"/>
-    </row>
-    <row r="42" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:18" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="37" t="s">
+      <c r="B41" s="48"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="48"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="48"/>
+      <c r="K41" s="48"/>
+      <c r="L41" s="48"/>
+      <c r="M41" s="48"/>
+      <c r="N41" s="48"/>
+      <c r="O41" s="48"/>
+      <c r="P41" s="48"/>
+      <c r="Q41" s="48"/>
+      <c r="R41" s="49"/>
+    </row>
+    <row r="42" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="52"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+      <c r="I42" s="52"/>
+      <c r="J42" s="52"/>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="52"/>
+      <c r="P42" s="52"/>
+      <c r="Q42" s="52"/>
+      <c r="R42" s="52"/>
+    </row>
+    <row r="43" spans="1:18" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="38"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="38"/>
-      <c r="F43" s="38"/>
-      <c r="G43" s="38"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
-      <c r="J43" s="38"/>
-      <c r="K43" s="38"/>
-      <c r="L43" s="38"/>
-      <c r="M43" s="38"/>
-      <c r="N43" s="38"/>
-      <c r="O43" s="38"/>
-      <c r="P43" s="38"/>
-      <c r="Q43" s="38"/>
-      <c r="R43" s="39"/>
-    </row>
-    <row r="44" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:18" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="37" t="s">
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="48"/>
+      <c r="L43" s="48"/>
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="48"/>
+      <c r="P43" s="48"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="49"/>
+    </row>
+    <row r="44" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="52"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="52"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="52"/>
+      <c r="P44" s="52"/>
+      <c r="Q44" s="52"/>
+      <c r="R44" s="52"/>
+    </row>
+    <row r="45" spans="1:18" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="38"/>
-      <c r="K45" s="38"/>
-      <c r="L45" s="38"/>
-      <c r="M45" s="38"/>
-      <c r="N45" s="38"/>
-      <c r="O45" s="38"/>
-      <c r="P45" s="38"/>
-      <c r="Q45" s="38"/>
-      <c r="R45" s="39"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
+      <c r="K45" s="48"/>
+      <c r="L45" s="48"/>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="48"/>
+      <c r="P45" s="48"/>
+      <c r="Q45" s="48"/>
+      <c r="R45" s="49"/>
+    </row>
+    <row r="46" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="52"/>
+      <c r="B46" s="52"/>
+      <c r="C46" s="52"/>
+      <c r="D46" s="52"/>
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="52"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="52"/>
+      <c r="K46" s="52"/>
+      <c r="L46" s="52"/>
+      <c r="M46" s="52"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="52"/>
+      <c r="P46" s="52"/>
+      <c r="Q46" s="52"/>
+      <c r="R46" s="52"/>
+    </row>
+    <row r="47" spans="1:18" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="48"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="48"/>
+      <c r="P47" s="48"/>
+      <c r="Q47" s="48"/>
+      <c r="R47" s="49"/>
+    </row>
+    <row r="48" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="52"/>
+      <c r="B48" s="52"/>
+      <c r="C48" s="52"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="K48" s="52"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="52"/>
+      <c r="P48" s="52"/>
+      <c r="Q48" s="52"/>
+      <c r="R48" s="52"/>
+    </row>
+    <row r="49" spans="1:18" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="48"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="48"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="48"/>
+      <c r="P49" s="48"/>
+      <c r="Q49" s="48"/>
+      <c r="R49" s="49"/>
+    </row>
+    <row r="50" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="53"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="53"/>
+      <c r="D50" s="53"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="53"/>
+      <c r="H50" s="53"/>
+      <c r="I50" s="53"/>
+      <c r="J50" s="53"/>
+      <c r="K50" s="53"/>
+      <c r="L50" s="53"/>
+      <c r="M50" s="53"/>
+      <c r="N50" s="53"/>
+      <c r="O50" s="53"/>
+      <c r="P50" s="53"/>
+      <c r="Q50" s="53"/>
+      <c r="R50" s="53"/>
+    </row>
+    <row r="51" spans="1:18" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="48"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="48"/>
+      <c r="K51" s="48"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="48"/>
+      <c r="P51" s="48"/>
+      <c r="Q51" s="48"/>
+      <c r="R51" s="49"/>
     </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A45:R45"/>
-    <mergeCell ref="R30:R32"/>
-    <mergeCell ref="A43:R43"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A41:R41"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="P30:P32"/>
-    <mergeCell ref="Q30:Q32"/>
+  <mergeCells count="30">
+    <mergeCell ref="A47:R47"/>
+    <mergeCell ref="A49:R49"/>
+    <mergeCell ref="A51:R51"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="F30:F32"/>
     <mergeCell ref="G30:G32"/>
@@ -1757,6 +1974,17 @@
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="D30:D32"/>
+    <mergeCell ref="A45:R45"/>
+    <mergeCell ref="R30:R32"/>
+    <mergeCell ref="A43:R43"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A41:R41"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="P30:P32"/>
+    <mergeCell ref="Q30:Q32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
IICE set flag added
</commit_message>
<xml_diff>
--- a/КУМП.xlsx
+++ b/КУМП.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>0x1</t>
   </si>
@@ -114,6 +114,12 @@
       </rPr>
       <t xml:space="preserve"> - 125°с).</t>
     </r>
+  </si>
+  <si>
+    <t>IICE ( Inter-Integrated Circuit Error) - Ошибка в работе интерфейса I2C.</t>
+  </si>
+  <si>
+    <t>IICE</t>
   </si>
 </sst>
 </file>
@@ -161,7 +167,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -622,11 +628,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -666,15 +771,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -693,43 +789,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -756,31 +841,57 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1082,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:R51"/>
+  <dimension ref="A2:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,69 +1208,69 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43"/>
-      <c r="M13" s="43"/>
-      <c r="N13" s="43"/>
-      <c r="O13" s="43"/>
-      <c r="P13" s="43"/>
-      <c r="Q13" s="44"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+      <c r="G13" s="37"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="37"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="37"/>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="38"/>
     </row>
     <row r="14" spans="1:17" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="36"/>
-      <c r="B14" s="39" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40"/>
-      <c r="O14" s="41"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="35"/>
       <c r="P14" s="1">
         <v>0</v>
       </c>
@@ -1369,166 +1480,170 @@
     </row>
     <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="31">
+      <c r="C30" s="28">
         <v>15</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="28">
         <v>14</v>
       </c>
-      <c r="E30" s="31">
+      <c r="E30" s="28">
         <v>13</v>
       </c>
-      <c r="F30" s="31">
+      <c r="F30" s="28">
         <v>12</v>
       </c>
-      <c r="G30" s="31">
+      <c r="G30" s="28">
         <v>11</v>
       </c>
-      <c r="H30" s="31">
+      <c r="H30" s="28">
         <v>10</v>
       </c>
-      <c r="I30" s="31">
+      <c r="I30" s="28">
         <v>9</v>
       </c>
-      <c r="J30" s="31">
+      <c r="J30" s="28">
         <v>8</v>
       </c>
-      <c r="K30" s="31">
+      <c r="K30" s="28">
         <v>7</v>
       </c>
-      <c r="L30" s="31">
+      <c r="L30" s="28">
         <v>6</v>
       </c>
-      <c r="M30" s="31">
+      <c r="M30" s="28">
         <v>5</v>
       </c>
-      <c r="N30" s="31">
+      <c r="N30" s="28">
         <v>4</v>
       </c>
-      <c r="O30" s="31">
+      <c r="O30" s="28">
         <v>3</v>
       </c>
-      <c r="P30" s="31">
+      <c r="P30" s="28">
         <v>2</v>
       </c>
-      <c r="Q30" s="31">
+      <c r="Q30" s="28">
         <v>1</v>
       </c>
-      <c r="R30" s="26">
+      <c r="R30" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
-      <c r="K31" s="33"/>
-      <c r="L31" s="33"/>
-      <c r="M31" s="33"/>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="27"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="43"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="46"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="34"/>
-      <c r="Q32" s="34"/>
-      <c r="R32" s="28"/>
-    </row>
-    <row r="33" spans="1:18" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A32" s="41"/>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
+      <c r="P32" s="30"/>
+      <c r="Q32" s="30"/>
+      <c r="R32" s="44"/>
+    </row>
+    <row r="33" spans="1:18" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="24" t="s">
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="M33" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="N33" s="50" t="s">
+      <c r="N33" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="O33" s="50" t="s">
+      <c r="O33" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="P33" s="50" t="s">
+      <c r="P33" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="Q33" s="15" t="s">
+      <c r="Q33" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="R33" s="16" t="s">
+      <c r="R33" s="55" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="21"/>
-      <c r="L34" s="21"/>
-      <c r="M34" s="25">
-        <v>0</v>
-      </c>
-      <c r="N34" s="51">
-        <v>0</v>
-      </c>
-      <c r="O34" s="51">
-        <v>0</v>
-      </c>
-      <c r="P34" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q34" s="17">
+      <c r="A34" s="45"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="47">
+        <v>0</v>
+      </c>
+      <c r="M34" s="48">
+        <v>0</v>
+      </c>
+      <c r="N34" s="49">
+        <v>0</v>
+      </c>
+      <c r="O34" s="49">
+        <v>0</v>
+      </c>
+      <c r="P34" s="49">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="50">
         <v>1</v>
       </c>
-      <c r="R34" s="13">
+      <c r="R34" s="51">
         <v>1</v>
       </c>
     </row>
@@ -1569,22 +1684,22 @@
       <c r="L35" s="11">
         <v>0</v>
       </c>
-      <c r="M35" s="22">
-        <v>0</v>
-      </c>
-      <c r="N35" s="22">
-        <v>0</v>
-      </c>
-      <c r="O35" s="22">
-        <v>0</v>
-      </c>
-      <c r="P35" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="22">
-        <v>0</v>
-      </c>
-      <c r="R35" s="23">
+      <c r="M35" s="19">
+        <v>0</v>
+      </c>
+      <c r="N35" s="19">
+        <v>0</v>
+      </c>
+      <c r="O35" s="19">
+        <v>0</v>
+      </c>
+      <c r="P35" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="19">
+        <v>0</v>
+      </c>
+      <c r="R35" s="20">
         <v>0</v>
       </c>
     </row>
@@ -1722,245 +1837,263 @@
     </row>
     <row r="40" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:18" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="47" t="s">
+      <c r="A41" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="48"/>
-      <c r="C41" s="48"/>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="48"/>
-      <c r="L41" s="48"/>
-      <c r="M41" s="48"/>
-      <c r="N41" s="48"/>
-      <c r="O41" s="48"/>
-      <c r="P41" s="48"/>
-      <c r="Q41" s="48"/>
-      <c r="R41" s="49"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="24"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="25"/>
     </row>
     <row r="42" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="52"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="52"/>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="52"/>
-      <c r="G42" s="52"/>
-      <c r="H42" s="52"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="52"/>
-      <c r="K42" s="52"/>
-      <c r="L42" s="52"/>
-      <c r="M42" s="52"/>
-      <c r="N42" s="52"/>
-      <c r="O42" s="52"/>
-      <c r="P42" s="52"/>
-      <c r="Q42" s="52"/>
-      <c r="R42" s="52"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="21"/>
+      <c r="R42" s="21"/>
     </row>
     <row r="43" spans="1:18" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="47" t="s">
+      <c r="A43" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
-      <c r="D43" s="48"/>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="48"/>
-      <c r="L43" s="48"/>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
-      <c r="R43" s="49"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="F43" s="24"/>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
+      <c r="K43" s="24"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
+      <c r="N43" s="24"/>
+      <c r="O43" s="24"/>
+      <c r="P43" s="24"/>
+      <c r="Q43" s="24"/>
+      <c r="R43" s="25"/>
     </row>
     <row r="44" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="52"/>
-      <c r="B44" s="52"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
-      <c r="F44" s="52"/>
-      <c r="G44" s="52"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
-      <c r="K44" s="52"/>
-      <c r="L44" s="52"/>
-      <c r="M44" s="52"/>
-      <c r="N44" s="52"/>
-      <c r="O44" s="52"/>
-      <c r="P44" s="52"/>
-      <c r="Q44" s="52"/>
-      <c r="R44" s="52"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="21"/>
+      <c r="Q44" s="21"/>
+      <c r="R44" s="21"/>
     </row>
     <row r="45" spans="1:18" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="47" t="s">
+      <c r="A45" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
-      <c r="K45" s="48"/>
-      <c r="L45" s="48"/>
-      <c r="M45" s="48"/>
-      <c r="N45" s="48"/>
-      <c r="O45" s="48"/>
-      <c r="P45" s="48"/>
-      <c r="Q45" s="48"/>
-      <c r="R45" s="49"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
+      <c r="K45" s="24"/>
+      <c r="L45" s="24"/>
+      <c r="M45" s="24"/>
+      <c r="N45" s="24"/>
+      <c r="O45" s="24"/>
+      <c r="P45" s="24"/>
+      <c r="Q45" s="24"/>
+      <c r="R45" s="25"/>
     </row>
     <row r="46" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="52"/>
-      <c r="B46" s="52"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="52"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="52"/>
-      <c r="H46" s="52"/>
-      <c r="I46" s="52"/>
-      <c r="J46" s="52"/>
-      <c r="K46" s="52"/>
-      <c r="L46" s="52"/>
-      <c r="M46" s="52"/>
-      <c r="N46" s="52"/>
-      <c r="O46" s="52"/>
-      <c r="P46" s="52"/>
-      <c r="Q46" s="52"/>
-      <c r="R46" s="52"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="21"/>
+      <c r="R46" s="21"/>
     </row>
     <row r="47" spans="1:18" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="47" t="s">
+      <c r="A47" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="48"/>
-      <c r="C47" s="48"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="48"/>
-      <c r="K47" s="48"/>
-      <c r="L47" s="48"/>
-      <c r="M47" s="48"/>
-      <c r="N47" s="48"/>
-      <c r="O47" s="48"/>
-      <c r="P47" s="48"/>
-      <c r="Q47" s="48"/>
-      <c r="R47" s="49"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24"/>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24"/>
+      <c r="K47" s="24"/>
+      <c r="L47" s="24"/>
+      <c r="M47" s="24"/>
+      <c r="N47" s="24"/>
+      <c r="O47" s="24"/>
+      <c r="P47" s="24"/>
+      <c r="Q47" s="24"/>
+      <c r="R47" s="25"/>
     </row>
     <row r="48" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="52"/>
-      <c r="B48" s="52"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="52"/>
-      <c r="F48" s="52"/>
-      <c r="G48" s="52"/>
-      <c r="H48" s="52"/>
-      <c r="I48" s="52"/>
-      <c r="J48" s="52"/>
-      <c r="K48" s="52"/>
-      <c r="L48" s="52"/>
-      <c r="M48" s="52"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="52"/>
-      <c r="P48" s="52"/>
-      <c r="Q48" s="52"/>
-      <c r="R48" s="52"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="21"/>
+      <c r="P48" s="21"/>
+      <c r="Q48" s="21"/>
+      <c r="R48" s="21"/>
     </row>
     <row r="49" spans="1:18" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="47" t="s">
+      <c r="A49" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="48"/>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="48"/>
-      <c r="K49" s="48"/>
-      <c r="L49" s="48"/>
-      <c r="M49" s="48"/>
-      <c r="N49" s="48"/>
-      <c r="O49" s="48"/>
-      <c r="P49" s="48"/>
-      <c r="Q49" s="48"/>
-      <c r="R49" s="49"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24"/>
+      <c r="K49" s="24"/>
+      <c r="L49" s="24"/>
+      <c r="M49" s="24"/>
+      <c r="N49" s="24"/>
+      <c r="O49" s="24"/>
+      <c r="P49" s="24"/>
+      <c r="Q49" s="24"/>
+      <c r="R49" s="25"/>
     </row>
     <row r="50" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="53"/>
-      <c r="B50" s="53"/>
-      <c r="C50" s="53"/>
-      <c r="D50" s="53"/>
-      <c r="E50" s="53"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="53"/>
-      <c r="H50" s="53"/>
-      <c r="I50" s="53"/>
-      <c r="J50" s="53"/>
-      <c r="K50" s="53"/>
-      <c r="L50" s="53"/>
-      <c r="M50" s="53"/>
-      <c r="N50" s="53"/>
-      <c r="O50" s="53"/>
-      <c r="P50" s="53"/>
-      <c r="Q50" s="53"/>
-      <c r="R50" s="53"/>
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="22"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="22"/>
+      <c r="K50" s="22"/>
+      <c r="L50" s="22"/>
+      <c r="M50" s="22"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
+      <c r="P50" s="22"/>
+      <c r="Q50" s="22"/>
+      <c r="R50" s="22"/>
     </row>
     <row r="51" spans="1:18" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="47" t="s">
+      <c r="A51" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B51" s="48"/>
-      <c r="C51" s="48"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48"/>
-      <c r="J51" s="48"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="48"/>
-      <c r="P51" s="48"/>
-      <c r="Q51" s="48"/>
-      <c r="R51" s="49"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
+      <c r="K51" s="24"/>
+      <c r="L51" s="24"/>
+      <c r="M51" s="24"/>
+      <c r="N51" s="24"/>
+      <c r="O51" s="24"/>
+      <c r="P51" s="24"/>
+      <c r="Q51" s="24"/>
+      <c r="R51" s="25"/>
+    </row>
+    <row r="52" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:18" ht="66" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
+      <c r="H53" s="24"/>
+      <c r="I53" s="24"/>
+      <c r="J53" s="24"/>
+      <c r="K53" s="24"/>
+      <c r="L53" s="24"/>
+      <c r="M53" s="24"/>
+      <c r="N53" s="24"/>
+      <c r="O53" s="24"/>
+      <c r="P53" s="24"/>
+      <c r="Q53" s="24"/>
+      <c r="R53" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
-    <mergeCell ref="A47:R47"/>
-    <mergeCell ref="A49:R49"/>
-    <mergeCell ref="A51:R51"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="G30:G32"/>
+  <mergeCells count="31">
+    <mergeCell ref="A53:R53"/>
     <mergeCell ref="B2:Q2"/>
     <mergeCell ref="H30:H32"/>
     <mergeCell ref="I30:I32"/>
@@ -1970,20 +2103,26 @@
     <mergeCell ref="M30:M32"/>
     <mergeCell ref="B14:O14"/>
     <mergeCell ref="B13:Q13"/>
-    <mergeCell ref="A30:A32"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="N30:N32"/>
+    <mergeCell ref="O30:O32"/>
+    <mergeCell ref="P30:P32"/>
+    <mergeCell ref="A47:R47"/>
+    <mergeCell ref="A49:R49"/>
+    <mergeCell ref="A51:R51"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="G30:G32"/>
+    <mergeCell ref="A30:A32"/>
     <mergeCell ref="A45:R45"/>
     <mergeCell ref="R30:R32"/>
     <mergeCell ref="A43:R43"/>
     <mergeCell ref="A33:A34"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="A41:R41"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="N30:N32"/>
-    <mergeCell ref="O30:O32"/>
-    <mergeCell ref="P30:P32"/>
     <mergeCell ref="Q30:Q32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>